<commit_message>
Entrega de escaletas para recursos en GRECO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17070" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="280">
   <si>
     <t>Asignatura</t>
   </si>
@@ -578,6 +578,18 @@
     <t>Varias opciones. Simplificar fracciones algebraicas con monomios; con polinomios; dar una simplificación equivocada y pedir al estudiante que lo identifique y explique. Dar rectángulos u otras figuras geométricas y pedir de dada el área, expresen mediante un cociente uno de los lados.  Dar un valor numérico y calcular el área finalmente.</t>
   </si>
   <si>
+    <t>Adiciona y sustrae frcciones algebraicas con el mimso denominador</t>
+  </si>
+  <si>
+    <t>Suma o resta fracciones algebraicas  con diferente denominador</t>
+  </si>
+  <si>
+    <t>Descarta valarees en el denominador</t>
+  </si>
+  <si>
+    <t>Ejercicios para identificar qué valores deben descartarse en el donominador de expresiones racionales</t>
+  </si>
+  <si>
     <t>La actividad se debe construir dando una fracción algebraica en la izquierda y en la derecha los valores numéricos que deben descartarse en el denominador. Deben proponerse fracciones que tengan dos valores para descartar y en la derecha proponer una por espacio.</t>
   </si>
   <si>
@@ -587,6 +599,9 @@
     <t>Proponer sumas y restas de fracciones algebraicas con el mismo denominador, siendo este un polinomio</t>
   </si>
   <si>
+    <t>Practica de las operaciones combinadas de sumas y restas de facciones algebraicas</t>
+  </si>
+  <si>
     <t>Sugerir actividades de operaciones combinadas de sumas y restas</t>
   </si>
   <si>
@@ -665,6 +680,9 @@
     <t>Competencias: las fracciones algebraicas en el sistema financiero</t>
   </si>
   <si>
+    <t>Actividad que muestra algunas fórmulas utilizadas por las entidades bancarias para calcular el valor de las cuotas que debe pagar una persona por un crédito.  Realizar preguntas para trabajar el pemsamiento crítico</t>
+  </si>
+  <si>
     <t>Actividad para relacionar dos o más monomios con su máximo común divisor</t>
   </si>
   <si>
@@ -677,21 +695,42 @@
     <t>Actividad para calcular el mínimo común múltiplo de dos polinomios</t>
   </si>
   <si>
+    <t>Actividad sobre El máximo común divisor y el mínimo común múltiplo</t>
+  </si>
+  <si>
     <t>Actividad para establecer expresiones racionales equivalentes</t>
   </si>
   <si>
     <t>Actividad para identificar equivalencias entre expresiones racionales, teniendo en cuenta el cambio de signo</t>
   </si>
   <si>
+    <t>Actividad para practicar la simplificación de epresiones racionales cuyos términos son monomios</t>
+  </si>
+  <si>
+    <t>Actividad para practicar la simplificación de epresiones racionales con polinomios en sus términos</t>
+  </si>
+  <si>
     <t>Actividad para completar expresiones y obtener fracciones equivalentes</t>
   </si>
   <si>
+    <t>Actividad para calcular la suma de fracciones algebracicas con monomios en el denominador</t>
+  </si>
+  <si>
+    <t>Actividad para calcular la suma de fracciones algebracicas con polinomios en el denominador</t>
+  </si>
+  <si>
     <t>Actividad para resolver situaciones en las cuales se apliquen la suma y la resta de fracciones algebraicas</t>
   </si>
   <si>
     <t>Actividad para obtener el producto de fracciones algebraicas</t>
   </si>
   <si>
+    <t>Actividad para analizar como reasolver situaciones de aplicación de la multiplicación y la división de expresiones racionales</t>
+  </si>
+  <si>
+    <t>Actividad sobre Las operaciones con fracciones algebraicas</t>
+  </si>
+  <si>
     <t>Actividad para simplificar fracciones complejas</t>
   </si>
   <si>
@@ -797,6 +836,9 @@
     <t>Mapa conceptual del tema Las fracciones algebraicas</t>
   </si>
   <si>
+    <t>Actividad que permite evaluar los concoimientos del estudiante sobre ell tema Las fracciones algebraicas</t>
+  </si>
+  <si>
     <t>Recurso F4-01</t>
   </si>
   <si>
@@ -821,46 +863,7 @@
     <t>Recurso M5A-03</t>
   </si>
   <si>
-    <t>Actividad sobre el máximo común divisor y el mínimo común múltiplo</t>
-  </si>
-  <si>
-    <t>Actividad para practicar la simplificación de expresiones racionales cuyos términos son monomios</t>
-  </si>
-  <si>
-    <t>Actividad para practicar la simplificación de expresiones racionales con polinomios en sus términos</t>
-  </si>
-  <si>
-    <t>Descarta valores en el denominador</t>
-  </si>
-  <si>
-    <t>Ejercicios para identificar qué valores deben descartarse en el denominador de expresiones racionales</t>
-  </si>
-  <si>
-    <t>Adiciona y sustrae fracciones algebraicas con el mismo denominador</t>
-  </si>
-  <si>
-    <t>Actividad para calcular la suma de fracciones algebraicas con polinomios en el denominador</t>
-  </si>
-  <si>
-    <t>Practica las operaciones combinadas de sumas y restas de facciones algebraicas</t>
-  </si>
-  <si>
-    <t>Actividad para calcular la suma de fracciones algebraicas con monomios en el denominador</t>
-  </si>
-  <si>
-    <t>Actividad para analizar como resolver situaciones de aplicación de la multiplicación y la división de expresiones racionales</t>
-  </si>
-  <si>
-    <t>Actividad sobre las operaciones con fracciones algebraicas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad que muestra algunas fórmulas utilizadas por las entidades bancarias para calcular el valor de las cuotas que debe pagar una persona por un crédito. </t>
-  </si>
-  <si>
-    <t>Actividad que permite evaluar los concoimientos del estudiante sobre el tema Las fracciones algebraicas</t>
-  </si>
-  <si>
-    <t>Adiciones y sustracciones de expresiones racionales con diferente denominador</t>
+    <t>Banco de contenidos</t>
   </si>
 </sst>
 </file>
@@ -1158,16 +1161,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1207,18 +1222,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1527,19 +1530,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="47.42578125" defaultRowHeight="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="12" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="26" style="12" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="26" customWidth="1"/>
     <col min="7" max="7" width="52.140625" style="12" customWidth="1"/>
     <col min="8" max="8" width="8.140625" style="28" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" style="26" customWidth="1"/>
@@ -1560,95 +1563,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="40" t="s">
+      <c r="N1" s="56"/>
+      <c r="O1" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="P1" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="Q1" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="58" t="s">
+      <c r="R1" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="57" t="s">
+      <c r="S1" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="T1" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="55" t="s">
+      <c r="U1" s="40" t="s">
         <v>90</v>
       </c>
       <c r="V1" s="36"/>
     </row>
     <row r="2" spans="1:22" s="6" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="47"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="51"/>
       <c r="M2" s="7" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="55"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="40"/>
       <c r="V2" s="36"/>
     </row>
     <row r="3" spans="1:22" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1698,16 +1701,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="31" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="S3" s="30" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="T3" s="32" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="U3" s="34" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1739,7 +1742,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>20</v>
@@ -1761,16 +1764,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S4" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T4" s="32" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="U4" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1802,7 +1805,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>20</v>
@@ -1824,16 +1827,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S5" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T5" s="32" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="U5" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1863,7 +1866,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>20</v>
@@ -1876,7 +1879,7 @@
         <v>22</v>
       </c>
       <c r="O6" s="13" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="P6" s="27" t="s">
         <v>19</v>
@@ -1885,16 +1888,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S6" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T6" s="32" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1924,7 +1927,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>20</v>
@@ -1946,16 +1949,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S7" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T7" s="32" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="U7" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1985,7 +1988,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>265</v>
+        <v>223</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>20</v>
@@ -2007,16 +2010,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S8" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T8" s="32" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="U8" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2044,7 +2047,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>20</v>
@@ -2066,16 +2069,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S9" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T9" s="32" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="U9" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2105,7 +2108,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>20</v>
@@ -2127,16 +2130,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S10" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T10" s="32" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="U10" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2166,7 +2169,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>266</v>
+        <v>226</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>20</v>
@@ -2188,16 +2191,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S11" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T11" s="32" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="U11" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2227,7 +2230,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>267</v>
+        <v>227</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>20</v>
@@ -2249,16 +2252,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S12" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T12" s="32" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="U12" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2288,7 +2291,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>20</v>
@@ -2310,16 +2313,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S13" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T13" s="32" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="U13" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2340,7 +2343,7 @@
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="3" t="s">
-        <v>268</v>
+        <v>186</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
@@ -2349,7 +2352,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>20</v>
@@ -2362,7 +2365,7 @@
         <v>29</v>
       </c>
       <c r="O14" s="13" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="P14" s="27" t="s">
         <v>19</v>
@@ -2371,16 +2374,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S14" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T14" s="32" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="U14" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2432,16 +2435,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="31" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="S15" s="30" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="T15" s="32" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="U15" s="34" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2493,16 +2496,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S16" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T16" s="32" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="U16" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2525,7 +2528,7 @@
         <v>165</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>270</v>
+        <v>184</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -2534,7 +2537,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>273</v>
+        <v>229</v>
       </c>
       <c r="K17" s="16" t="s">
         <v>20</v>
@@ -2547,7 +2550,7 @@
         <v>39</v>
       </c>
       <c r="O17" s="13" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="P17" s="27" t="s">
         <v>19</v>
@@ -2556,16 +2559,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S17" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T17" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="U17" s="34" t="s">
         <v>243</v>
-      </c>
-      <c r="U17" s="34" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2586,7 +2589,7 @@
         <v>166</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>278</v>
+        <v>185</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -2595,7 +2598,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>271</v>
+        <v>230</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>20</v>
@@ -2608,7 +2611,7 @@
         <v>39</v>
       </c>
       <c r="O18" s="13" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="P18" s="27" t="s">
         <v>19</v>
@@ -2617,16 +2620,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S18" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T18" s="32" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="U18" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2654,7 +2657,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>272</v>
+        <v>191</v>
       </c>
       <c r="K19" s="16" t="s">
         <v>20</v>
@@ -2667,7 +2670,7 @@
         <v>29</v>
       </c>
       <c r="O19" s="13" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="P19" s="27" t="s">
         <v>20</v>
@@ -2676,16 +2679,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S19" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T19" s="32" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="U19" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2713,7 +2716,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>20</v>
@@ -2726,7 +2729,7 @@
         <v>39</v>
       </c>
       <c r="O20" s="13" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="P20" s="27" t="s">
         <v>20</v>
@@ -2735,16 +2738,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S20" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T20" s="32" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="U20" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2772,7 +2775,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>20</v>
@@ -2785,7 +2788,7 @@
       </c>
       <c r="N21" s="18"/>
       <c r="O21" s="13" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="P21" s="27" t="s">
         <v>19</v>
@@ -2794,16 +2797,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S21" s="30" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="T21" s="32" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="U21" s="34" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2831,7 +2834,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>20</v>
@@ -2844,7 +2847,7 @@
         <v>121</v>
       </c>
       <c r="O22" s="13" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="P22" s="27" t="s">
         <v>19</v>
@@ -2853,16 +2856,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S22" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T22" s="32" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="U22" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2892,7 +2895,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>20</v>
@@ -2905,7 +2908,7 @@
         <v>39</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="P23" s="27" t="s">
         <v>19</v>
@@ -2914,16 +2917,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S23" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T23" s="32" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="U23" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2953,7 +2956,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>20</v>
@@ -2966,7 +2969,7 @@
         <v>40</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="P24" s="27" t="s">
         <v>20</v>
@@ -2975,16 +2978,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S24" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T24" s="32" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="U24" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3014,7 +3017,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>20</v>
@@ -3027,7 +3030,7 @@
         <v>39</v>
       </c>
       <c r="O25" s="13" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="P25" s="27" t="s">
         <v>19</v>
@@ -3036,16 +3039,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S25" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T25" s="32" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="U25" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3075,7 +3078,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>20</v>
@@ -3088,7 +3091,7 @@
         <v>33</v>
       </c>
       <c r="O26" s="13" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="P26" s="27" t="s">
         <v>19</v>
@@ -3097,16 +3100,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S26" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T26" s="32" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="U26" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3136,7 +3139,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="K27" s="16" t="s">
         <v>20</v>
@@ -3149,7 +3152,7 @@
         <v>39</v>
       </c>
       <c r="O27" s="13" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="P27" s="27" t="s">
         <v>19</v>
@@ -3158,16 +3161,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S27" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T27" s="32" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="U27" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3197,7 +3200,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="K28" s="16" t="s">
         <v>20</v>
@@ -3210,7 +3213,7 @@
       </c>
       <c r="N28" s="18"/>
       <c r="O28" s="13" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="P28" s="27" t="s">
         <v>19</v>
@@ -3219,16 +3222,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="31" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="S28" s="30" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="T28" s="32" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="U28" s="34" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3258,7 +3261,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="22" t="s">
-        <v>274</v>
+        <v>233</v>
       </c>
       <c r="K29" s="16" t="s">
         <v>20</v>
@@ -3271,7 +3274,7 @@
         <v>39</v>
       </c>
       <c r="O29" s="13" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="P29" s="27" t="s">
         <v>19</v>
@@ -3280,16 +3283,16 @@
         <v>6</v>
       </c>
       <c r="R29" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S29" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T29" s="32" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="U29" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3313,7 +3316,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>275</v>
+        <v>234</v>
       </c>
       <c r="K30" s="16" t="s">
         <v>20</v>
@@ -3326,7 +3329,7 @@
         <v>52</v>
       </c>
       <c r="O30" s="13" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="P30" s="27" t="s">
         <v>19</v>
@@ -3335,16 +3338,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S30" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T30" s="32" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="U30" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3372,7 +3375,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="K31" s="16" t="s">
         <v>20</v>
@@ -3385,7 +3388,7 @@
       </c>
       <c r="N31" s="18"/>
       <c r="O31" s="13" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="P31" s="27" t="s">
         <v>19</v>
@@ -3394,16 +3397,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S31" s="30" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="T31" s="32" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="U31" s="34" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3431,7 +3434,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="K32" s="16" t="s">
         <v>20</v>
@@ -3444,7 +3447,7 @@
         <v>39</v>
       </c>
       <c r="O32" s="13" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="P32" s="27" t="s">
         <v>19</v>
@@ -3453,16 +3456,16 @@
         <v>6</v>
       </c>
       <c r="R32" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S32" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T32" s="32" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="U32" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3492,7 +3495,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="K33" s="16" t="s">
         <v>20</v>
@@ -3505,7 +3508,7 @@
         <v>52</v>
       </c>
       <c r="O33" s="13" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="P33" s="27" t="s">
         <v>19</v>
@@ -3514,16 +3517,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S33" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T33" s="32" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="U33" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3542,7 +3545,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="13"/>
       <c r="G34" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="H34" s="27">
         <v>32</v>
@@ -3551,7 +3554,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>276</v>
+        <v>218</v>
       </c>
       <c r="K34" s="16" t="s">
         <v>20</v>
@@ -3569,16 +3572,16 @@
         <v>6</v>
       </c>
       <c r="R34" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S34" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T34" s="32" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="U34" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3604,7 +3607,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="22" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="K35" s="16" t="s">
         <v>20</v>
@@ -3643,7 +3646,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="K36" s="16" t="s">
         <v>20</v>
@@ -3661,16 +3664,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="S36" s="30" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="T36" s="32" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="U36" s="34" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3683,7 +3686,9 @@
       <c r="C37" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="11"/>
+      <c r="D37" s="11" t="s">
+        <v>279</v>
+      </c>
       <c r="E37" s="9"/>
       <c r="F37" s="13"/>
       <c r="G37" s="3"/>
@@ -3693,7 +3698,9 @@
       <c r="K37" s="16"/>
       <c r="L37" s="17"/>
       <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
+      <c r="N37" s="18" t="s">
+        <v>53</v>
+      </c>
       <c r="O37" s="13"/>
       <c r="P37" s="27"/>
       <c r="Q37" s="30"/>
@@ -4605,12 +4612,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4625,6 +4626,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revisión escaletas grado 6
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
-    <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
+    <sheet name="DATOS" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="284">
   <si>
     <t>Asignatura</t>
   </si>
@@ -864,6 +864,18 @@
   </si>
   <si>
     <t>Banco de contenidos</t>
+  </si>
+  <si>
+    <t>m101A</t>
+  </si>
+  <si>
+    <t>Miguel Muñoz</t>
+  </si>
+  <si>
+    <t>Joan Flórez</t>
+  </si>
+  <si>
+    <t>Recurso M101AP-01</t>
   </si>
 </sst>
 </file>
@@ -923,7 +935,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1000,6 +1012,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFABF8F"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1084,7 +1108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1224,6 +1248,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1530,9 +1556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q38" sqref="Q38"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W40" sqref="W40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="47.42578125" defaultRowHeight="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1558,7 +1584,7 @@
     <col min="19" max="19" width="12.7109375" style="12" customWidth="1"/>
     <col min="20" max="20" width="20.140625" style="12" customWidth="1"/>
     <col min="21" max="21" width="13.140625" style="12" customWidth="1"/>
-    <col min="22" max="22" width="47.42578125" style="37"/>
+    <col min="22" max="22" width="16.7109375" style="37" customWidth="1"/>
     <col min="23" max="16384" width="47.42578125" style="12"/>
   </cols>
   <sheetData>
@@ -1712,6 +1738,9 @@
       <c r="U3" s="34" t="s">
         <v>239</v>
       </c>
+      <c r="V3" s="60" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="4" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -1775,6 +1804,9 @@
       <c r="U4" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V4" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="5" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
@@ -1838,6 +1870,9 @@
       <c r="U5" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V5" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="6" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
@@ -1899,6 +1934,9 @@
       <c r="U6" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V6" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="7" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
@@ -1960,6 +1998,9 @@
       <c r="U7" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V7" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="8" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
@@ -1998,7 +2039,7 @@
       </c>
       <c r="M8" s="18"/>
       <c r="N8" s="18" t="s">
-        <v>52</v>
+        <v>280</v>
       </c>
       <c r="O8" s="13" t="s">
         <v>174</v>
@@ -2020,6 +2061,9 @@
       </c>
       <c r="U8" s="34" t="s">
         <v>243</v>
+      </c>
+      <c r="V8" s="59" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2080,6 +2124,9 @@
       <c r="U9" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V9" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="10" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -2141,6 +2188,9 @@
       <c r="U10" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V10" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="11" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -2202,6 +2252,9 @@
       <c r="U11" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V11" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="12" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -2263,6 +2316,9 @@
       <c r="U12" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V12" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="13" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -2324,6 +2380,9 @@
       <c r="U13" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V13" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="14" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -2385,6 +2444,9 @@
       <c r="U14" s="34" t="s">
         <v>243</v>
       </c>
+      <c r="V14" s="59" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="15" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -2446,6 +2508,9 @@
       <c r="U15" s="34" t="s">
         <v>239</v>
       </c>
+      <c r="V15" s="60" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="16" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
@@ -2484,7 +2549,7 @@
       </c>
       <c r="M16" s="18"/>
       <c r="N16" s="18" t="s">
-        <v>52</v>
+        <v>280</v>
       </c>
       <c r="O16" s="13" t="s">
         <v>183</v>
@@ -2507,8 +2572,11 @@
       <c r="U16" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V16" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -2570,8 +2638,11 @@
       <c r="U17" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V17" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
@@ -2631,8 +2702,11 @@
       <c r="U18" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V18" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
@@ -2690,8 +2764,11 @@
       <c r="U19" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V19" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
@@ -2749,8 +2826,11 @@
       <c r="U20" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V20" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
@@ -2808,8 +2888,11 @@
       <c r="U21" s="34" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V21" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>15</v>
       </c>
@@ -2867,8 +2950,11 @@
       <c r="U22" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V22" s="59" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
@@ -2928,8 +3014,11 @@
       <c r="U23" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V23" s="59" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
@@ -2989,8 +3078,11 @@
       <c r="U24" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V24" s="59" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
@@ -3050,8 +3142,11 @@
       <c r="U25" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V25" s="59" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
@@ -3111,8 +3206,11 @@
       <c r="U26" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V26" s="59" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>15</v>
       </c>
@@ -3172,8 +3270,11 @@
       <c r="U27" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V27" s="59" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>15</v>
       </c>
@@ -3233,8 +3334,11 @@
       <c r="U28" s="34" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V28" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>15</v>
       </c>
@@ -3294,8 +3398,11 @@
       <c r="U29" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V29" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -3326,7 +3433,7 @@
       </c>
       <c r="M30" s="18"/>
       <c r="N30" s="18" t="s">
-        <v>52</v>
+        <v>280</v>
       </c>
       <c r="O30" s="13" t="s">
         <v>210</v>
@@ -3349,8 +3456,11 @@
       <c r="U30" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V30" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>15</v>
       </c>
@@ -3408,8 +3518,11 @@
       <c r="U31" s="34" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V31" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>15</v>
       </c>
@@ -3467,8 +3580,11 @@
       <c r="U32" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V32" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>15</v>
       </c>
@@ -3528,8 +3644,11 @@
       <c r="U33" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V33" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>15</v>
       </c>
@@ -3583,8 +3702,11 @@
       <c r="U34" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V34" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>15</v>
       </c>
@@ -3622,8 +3744,11 @@
       <c r="S35" s="30"/>
       <c r="T35" s="33"/>
       <c r="U35" s="34"/>
-    </row>
-    <row r="36" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V35" s="59" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>15</v>
       </c>
@@ -3675,8 +3800,11 @@
       <c r="U36" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V36" s="59" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>15</v>
       </c>
@@ -3703,13 +3831,26 @@
       </c>
       <c r="O37" s="13"/>
       <c r="P37" s="27"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="31"/>
-      <c r="S37" s="30"/>
-      <c r="T37" s="33"/>
-      <c r="U37" s="34"/>
-    </row>
-    <row r="38" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q37" s="30">
+        <v>7</v>
+      </c>
+      <c r="R37" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="S37" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="T37" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="U37" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="V37" s="60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10"/>
@@ -3732,7 +3873,7 @@
       <c r="T38" s="21"/>
       <c r="U38" s="35"/>
     </row>
-    <row r="39" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10"/>
@@ -3755,7 +3896,7 @@
       <c r="T39" s="21"/>
       <c r="U39" s="35"/>
     </row>
-    <row r="40" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="24"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10"/>
@@ -3778,7 +3919,7 @@
       <c r="T40" s="21"/>
       <c r="U40" s="35"/>
     </row>
-    <row r="41" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="24"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10"/>
@@ -3801,7 +3942,7 @@
       <c r="T41" s="21"/>
       <c r="U41" s="35"/>
     </row>
-    <row r="42" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="24"/>
       <c r="B42" s="9"/>
       <c r="C42" s="10"/>
@@ -3824,7 +3965,7 @@
       <c r="T42" s="21"/>
       <c r="U42" s="35"/>
     </row>
-    <row r="43" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="24"/>
       <c r="B43" s="9"/>
       <c r="C43" s="10"/>
@@ -3847,7 +3988,7 @@
       <c r="T43" s="21"/>
       <c r="U43" s="35"/>
     </row>
-    <row r="44" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="24"/>
       <c r="B44" s="9"/>
       <c r="C44" s="10"/>
@@ -3870,7 +4011,7 @@
       <c r="T44" s="21"/>
       <c r="U44" s="35"/>
     </row>
-    <row r="45" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="24"/>
       <c r="B45" s="9"/>
       <c r="C45" s="10"/>
@@ -3893,7 +4034,7 @@
       <c r="T45" s="21"/>
       <c r="U45" s="35"/>
     </row>
-    <row r="46" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="24"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10"/>
@@ -3916,7 +4057,7 @@
       <c r="T46" s="21"/>
       <c r="U46" s="35"/>
     </row>
-    <row r="47" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="24"/>
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
@@ -3939,7 +4080,7 @@
       <c r="T47" s="21"/>
       <c r="U47" s="35"/>
     </row>
-    <row r="48" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="24"/>
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
@@ -4678,8 +4819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O133"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5402,7 +5543,7 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="1" t="s">
-        <v>52</v>
+        <v>280</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -6609,7 +6750,6 @@
       <c r="L133" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="duoSM2/GxQjtLYdKATObDXlCVo4hGTfBwoNvMjp43nnNpPoG3zCSd176iq0wGi+jtJb5dBDCNBT69VkNoNId2w==" saltValue="Qr58l5OQKNMYax0PAe5thA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I134:I1283">
       <formula1>$B$1:$B$7</formula1>

</xml_diff>

<commit_message>
Asignación de recursos mat 8 T5 en greco
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="285">
   <si>
     <t>Asignatura</t>
   </si>
@@ -872,10 +872,13 @@
     <t>Miguel Muñoz</t>
   </si>
   <si>
-    <t>Joan Flórez</t>
-  </si>
-  <si>
     <t>Recurso M101AP-01</t>
+  </si>
+  <si>
+    <t>Andrea Sabogal</t>
+  </si>
+  <si>
+    <t>Andrea Santos</t>
   </si>
 </sst>
 </file>
@@ -935,7 +938,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1026,6 +1029,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -1108,7 +1117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1185,28 +1194,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1248,8 +1247,19 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1557,8 +1567,8 @@
   <dimension ref="A1:V119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W40" sqref="W40"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="47.42578125" defaultRowHeight="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1589,95 +1599,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="I1" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="56" t="s">
+      <c r="M1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="38" t="s">
+      <c r="N1" s="54"/>
+      <c r="O1" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="42" t="s">
+      <c r="Q1" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="43" t="s">
+      <c r="R1" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="42" t="s">
+      <c r="S1" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="U1" s="57" t="s">
         <v>90</v>
       </c>
       <c r="V1" s="36"/>
     </row>
     <row r="2" spans="1:22" s="6" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="51"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="49"/>
       <c r="M2" s="7" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="40"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="36"/>
     </row>
     <row r="3" spans="1:22" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1738,8 +1748,8 @@
       <c r="U3" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="V3" s="60" t="s">
-        <v>282</v>
+      <c r="V3" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1804,7 +1814,7 @@
       <c r="U4" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V4" s="59" t="s">
+      <c r="V4" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -1870,7 +1880,7 @@
       <c r="U5" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V5" s="59" t="s">
+      <c r="V5" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -1934,7 +1944,7 @@
       <c r="U6" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V6" s="59" t="s">
+      <c r="V6" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -1998,7 +2008,7 @@
       <c r="U7" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V7" s="59" t="s">
+      <c r="V7" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2062,7 +2072,7 @@
       <c r="U8" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V8" s="59" t="s">
+      <c r="V8" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2124,7 +2134,7 @@
       <c r="U9" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V9" s="59" t="s">
+      <c r="V9" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2188,7 +2198,7 @@
       <c r="U10" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="59" t="s">
+      <c r="V10" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2252,7 +2262,7 @@
       <c r="U11" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V11" s="59" t="s">
+      <c r="V11" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2316,7 +2326,7 @@
       <c r="U12" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V12" s="59" t="s">
+      <c r="V12" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2380,7 +2390,7 @@
       <c r="U13" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V13" s="59" t="s">
+      <c r="V13" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2444,7 +2454,7 @@
       <c r="U14" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V14" s="59" t="s">
+      <c r="V14" s="38" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2508,8 +2518,8 @@
       <c r="U15" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="V15" s="60" t="s">
-        <v>282</v>
+      <c r="V15" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2572,8 +2582,8 @@
       <c r="U16" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V16" s="60" t="s">
-        <v>282</v>
+      <c r="V16" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2638,8 +2648,8 @@
       <c r="U17" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V17" s="60" t="s">
-        <v>282</v>
+      <c r="V17" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2702,8 +2712,8 @@
       <c r="U18" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V18" s="60" t="s">
-        <v>282</v>
+      <c r="V18" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2764,8 +2774,8 @@
       <c r="U19" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V19" s="60" t="s">
-        <v>282</v>
+      <c r="V19" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2826,8 +2836,8 @@
       <c r="U20" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V20" s="60" t="s">
-        <v>282</v>
+      <c r="V20" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2888,8 +2898,8 @@
       <c r="U21" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="V21" s="60" t="s">
-        <v>282</v>
+      <c r="V21" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2950,8 +2960,8 @@
       <c r="U22" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V22" s="59" t="s">
-        <v>281</v>
+      <c r="V22" s="61" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3014,8 +3024,8 @@
       <c r="U23" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V23" s="59" t="s">
-        <v>281</v>
+      <c r="V23" s="61" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3078,8 +3088,8 @@
       <c r="U24" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V24" s="59" t="s">
-        <v>281</v>
+      <c r="V24" s="61" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3142,8 +3152,8 @@
       <c r="U25" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V25" s="59" t="s">
-        <v>281</v>
+      <c r="V25" s="61" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3206,8 +3216,8 @@
       <c r="U26" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V26" s="59" t="s">
-        <v>281</v>
+      <c r="V26" s="61" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3270,8 +3280,8 @@
       <c r="U27" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V27" s="59" t="s">
-        <v>281</v>
+      <c r="V27" s="61" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3334,8 +3344,8 @@
       <c r="U28" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="V28" s="60" t="s">
-        <v>282</v>
+      <c r="V28" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3398,8 +3408,8 @@
       <c r="U29" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V29" s="60" t="s">
-        <v>282</v>
+      <c r="V29" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3456,8 +3466,8 @@
       <c r="U30" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V30" s="60" t="s">
-        <v>282</v>
+      <c r="V30" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3518,8 +3528,8 @@
       <c r="U31" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="V31" s="60" t="s">
-        <v>282</v>
+      <c r="V31" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3580,8 +3590,8 @@
       <c r="U32" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V32" s="60" t="s">
-        <v>282</v>
+      <c r="V32" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3644,8 +3654,8 @@
       <c r="U33" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V33" s="60" t="s">
-        <v>282</v>
+      <c r="V33" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3702,8 +3712,8 @@
       <c r="U34" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V34" s="60" t="s">
-        <v>282</v>
+      <c r="V34" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3744,8 +3754,8 @@
       <c r="S35" s="30"/>
       <c r="T35" s="33"/>
       <c r="U35" s="34"/>
-      <c r="V35" s="59" t="s">
-        <v>281</v>
+      <c r="V35" s="61" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3800,8 +3810,8 @@
       <c r="U36" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V36" s="59" t="s">
-        <v>281</v>
+      <c r="V36" s="61" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3841,13 +3851,13 @@
         <v>241</v>
       </c>
       <c r="T37" s="32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="U37" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="V37" s="60" t="s">
-        <v>282</v>
+      <c r="V37" s="39" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4753,6 +4763,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4767,12 +4783,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se quita recurso M102ab de cuaderno de etudio
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1352,28 +1352,30 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1415,20 +1417,18 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1735,9 +1735,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y36" sqref="Y36"/>
+      <selection pane="bottomLeft" activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="47.42578125" defaultRowHeight="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1770,25 +1770,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="3" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="45" t="s">
         <v>112</v>
       </c>
       <c r="F1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="41" t="s">
@@ -1797,68 +1797,68 @@
       <c r="I1" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="35" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="R1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="38" t="s">
+      <c r="T1" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="58" t="s">
         <v>90</v>
       </c>
       <c r="V1" s="13"/>
     </row>
     <row r="2" spans="1:25" s="3" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="44"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="42"/>
-      <c r="G2" s="48"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="48"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="37"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="58"/>
       <c r="V2" s="13"/>
       <c r="W2" s="22" t="s">
         <v>270</v>
@@ -1919,19 +1919,19 @@
       <c r="S3" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="T3" s="56" t="s">
+      <c r="T3" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="U3" s="57" t="s">
+      <c r="U3" s="36" t="s">
         <v>223</v>
       </c>
       <c r="V3" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W3" s="61">
+      <c r="W3" s="40">
         <v>42326</v>
       </c>
-      <c r="X3" s="61">
+      <c r="X3" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -1954,7 +1954,7 @@
       <c r="F4" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="37" t="s">
         <v>131</v>
       </c>
       <c r="H4" s="24">
@@ -1991,10 +1991,10 @@
       <c r="S4" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T4" s="56" t="s">
+      <c r="T4" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="U4" s="57" t="s">
+      <c r="U4" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V4" s="26" t="s">
@@ -2059,16 +2059,16 @@
       <c r="S5" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T5" s="56" t="s">
+      <c r="T5" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="U5" s="57" t="s">
+      <c r="U5" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V5" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="W5" s="61">
+      <c r="W5" s="40">
         <v>42320</v>
       </c>
       <c r="X5" s="10"/>
@@ -2090,7 +2090,7 @@
       <c r="F6" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="37" t="s">
         <v>272</v>
       </c>
       <c r="H6" s="24">
@@ -2127,16 +2127,16 @@
       <c r="S6" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T6" s="56" t="s">
+      <c r="T6" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="U6" s="57" t="s">
+      <c r="U6" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V6" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="W6" s="61">
+      <c r="W6" s="40">
         <v>42320</v>
       </c>
       <c r="X6" s="10"/>
@@ -2195,16 +2195,16 @@
       <c r="S7" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T7" s="56" t="s">
+      <c r="T7" s="35" t="s">
         <v>230</v>
       </c>
-      <c r="U7" s="57" t="s">
+      <c r="U7" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V7" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="W7" s="61">
+      <c r="W7" s="40">
         <v>42320</v>
       </c>
       <c r="X7" s="10"/>
@@ -2262,16 +2262,16 @@
       <c r="S8" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T8" s="56" t="s">
+      <c r="T8" s="35" t="s">
         <v>231</v>
       </c>
-      <c r="U8" s="57" t="s">
+      <c r="U8" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V8" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="W8" s="61">
+      <c r="W8" s="40">
         <v>42334</v>
       </c>
       <c r="X8" s="10"/>
@@ -2328,19 +2328,19 @@
       <c r="S9" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T9" s="56" t="s">
+      <c r="T9" s="35" t="s">
         <v>232</v>
       </c>
-      <c r="U9" s="57" t="s">
+      <c r="U9" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V9" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="W9" s="61">
+      <c r="W9" s="40">
         <v>42354</v>
       </c>
-      <c r="X9" s="61">
+      <c r="X9" s="40">
         <v>42334</v>
       </c>
     </row>
@@ -2398,19 +2398,19 @@
       <c r="S10" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T10" s="56" t="s">
+      <c r="T10" s="35" t="s">
         <v>233</v>
       </c>
-      <c r="U10" s="57" t="s">
+      <c r="U10" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V10" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="W10" s="61">
+      <c r="W10" s="40">
         <v>42354</v>
       </c>
-      <c r="X10" s="61">
+      <c r="X10" s="40">
         <v>42334</v>
       </c>
     </row>
@@ -2440,7 +2440,7 @@
       <c r="I11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="38" t="s">
         <v>213</v>
       </c>
       <c r="K11" s="25" t="s">
@@ -2468,19 +2468,19 @@
       <c r="S11" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T11" s="56" t="s">
+      <c r="T11" s="35" t="s">
         <v>234</v>
       </c>
-      <c r="U11" s="57" t="s">
+      <c r="U11" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V11" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="W11" s="61">
+      <c r="W11" s="40">
         <v>42354</v>
       </c>
-      <c r="X11" s="61">
+      <c r="X11" s="40">
         <v>42334</v>
       </c>
     </row>
@@ -2538,19 +2538,19 @@
       <c r="S12" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T12" s="56" t="s">
+      <c r="T12" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="U12" s="57" t="s">
+      <c r="U12" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V12" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="W12" s="61">
+      <c r="W12" s="40">
         <v>42334</v>
       </c>
-      <c r="X12" s="61">
+      <c r="X12" s="40">
         <v>42334</v>
       </c>
     </row>
@@ -2608,19 +2608,19 @@
       <c r="S13" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T13" s="56" t="s">
+      <c r="T13" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="U13" s="57" t="s">
+      <c r="U13" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V13" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="W13" s="61">
+      <c r="W13" s="40">
         <v>42334</v>
       </c>
-      <c r="X13" s="61">
+      <c r="X13" s="40">
         <v>42334</v>
       </c>
     </row>
@@ -2678,17 +2678,17 @@
       <c r="S14" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T14" s="56" t="s">
+      <c r="T14" s="35" t="s">
         <v>237</v>
       </c>
-      <c r="U14" s="57" t="s">
+      <c r="U14" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V14" s="26" t="s">
         <v>265</v>
       </c>
       <c r="W14" s="10"/>
-      <c r="X14" s="61">
+      <c r="X14" s="40">
         <v>42338</v>
       </c>
     </row>
@@ -2746,19 +2746,19 @@
       <c r="S15" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="T15" s="56" t="s">
+      <c r="T15" s="35" t="s">
         <v>238</v>
       </c>
-      <c r="U15" s="57" t="s">
+      <c r="U15" s="36" t="s">
         <v>223</v>
       </c>
       <c r="V15" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W15" s="61">
+      <c r="W15" s="40">
         <v>42326</v>
       </c>
-      <c r="X15" s="61">
+      <c r="X15" s="40">
         <v>42327</v>
       </c>
       <c r="Y15" s="32"/>
@@ -2817,17 +2817,17 @@
       <c r="S16" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T16" s="56" t="s">
+      <c r="T16" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="U16" s="57" t="s">
+      <c r="U16" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V16" s="26" t="s">
         <v>267</v>
       </c>
       <c r="W16" s="10"/>
-      <c r="X16" s="61">
+      <c r="X16" s="40">
         <v>42321</v>
       </c>
       <c r="Y16" s="33"/>
@@ -2888,19 +2888,19 @@
       <c r="S17" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T17" s="56" t="s">
+      <c r="T17" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="U17" s="57" t="s">
+      <c r="U17" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V17" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W17" s="61">
+      <c r="W17" s="40">
         <v>42352</v>
       </c>
-      <c r="X17" s="61">
+      <c r="X17" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -2958,19 +2958,19 @@
       <c r="S18" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T18" s="56" t="s">
+      <c r="T18" s="35" t="s">
         <v>241</v>
       </c>
-      <c r="U18" s="57" t="s">
+      <c r="U18" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V18" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W18" s="61">
+      <c r="W18" s="40">
         <v>42352</v>
       </c>
-      <c r="X18" s="61">
+      <c r="X18" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -3026,19 +3026,19 @@
       <c r="S19" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T19" s="56" t="s">
+      <c r="T19" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="U19" s="57" t="s">
+      <c r="U19" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V19" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W19" s="61">
+      <c r="W19" s="40">
         <v>42352</v>
       </c>
-      <c r="X19" s="61">
+      <c r="X19" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -3094,19 +3094,19 @@
       <c r="S20" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T20" s="56" t="s">
+      <c r="T20" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="U20" s="57" t="s">
+      <c r="U20" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V20" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W20" s="61">
+      <c r="W20" s="40">
         <v>42352</v>
       </c>
-      <c r="X20" s="61">
+      <c r="X20" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -3162,19 +3162,19 @@
       <c r="S21" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="T21" s="56" t="s">
+      <c r="T21" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="U21" s="57" t="s">
+      <c r="U21" s="36" t="s">
         <v>246</v>
       </c>
       <c r="V21" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W21" s="61">
+      <c r="W21" s="40">
         <v>42326</v>
       </c>
-      <c r="X21" s="61">
+      <c r="X21" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="26"/>
-      <c r="G22" s="60" t="s">
+      <c r="G22" s="39" t="s">
         <v>285</v>
       </c>
       <c r="H22" s="24">
@@ -3202,7 +3202,7 @@
       <c r="I22" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="38" t="s">
         <v>286</v>
       </c>
       <c r="K22" s="25" t="s">
@@ -3219,7 +3219,7 @@
         <v>184</v>
       </c>
       <c r="P22" s="24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q22" s="24">
         <v>6</v>
@@ -3230,17 +3230,17 @@
       <c r="S22" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T22" s="56" t="s">
+      <c r="T22" s="35" t="s">
         <v>247</v>
       </c>
-      <c r="U22" s="57" t="s">
+      <c r="U22" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V22" s="26" t="s">
         <v>268</v>
       </c>
       <c r="W22" s="10"/>
-      <c r="X22" s="61">
+      <c r="X22" s="40">
         <v>42338</v>
       </c>
     </row>
@@ -3298,17 +3298,17 @@
       <c r="S23" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T23" s="56" t="s">
+      <c r="T23" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="U23" s="57" t="s">
+      <c r="U23" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V23" s="26" t="s">
         <v>268</v>
       </c>
       <c r="W23" s="10"/>
-      <c r="X23" s="61">
+      <c r="X23" s="40">
         <v>42328</v>
       </c>
     </row>
@@ -3366,16 +3366,16 @@
       <c r="S24" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T24" s="56" t="s">
+      <c r="T24" s="35" t="s">
         <v>249</v>
       </c>
-      <c r="U24" s="57" t="s">
+      <c r="U24" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V24" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="W24" s="61">
+      <c r="W24" s="40">
         <v>42322</v>
       </c>
       <c r="X24" s="10" t="s">
@@ -3436,19 +3436,19 @@
       <c r="S25" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T25" s="56" t="s">
+      <c r="T25" s="35" t="s">
         <v>250</v>
       </c>
-      <c r="U25" s="57" t="s">
+      <c r="U25" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V25" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="W25" s="61">
+      <c r="W25" s="40">
         <v>42333</v>
       </c>
-      <c r="X25" s="61">
+      <c r="X25" s="40">
         <v>42333</v>
       </c>
       <c r="Y25" s="34"/>
@@ -3507,19 +3507,19 @@
       <c r="S26" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T26" s="56" t="s">
+      <c r="T26" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="U26" s="57" t="s">
+      <c r="U26" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V26" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="W26" s="61">
+      <c r="W26" s="40">
         <v>42321</v>
       </c>
-      <c r="X26" s="61">
+      <c r="X26" s="40">
         <v>42321</v>
       </c>
     </row>
@@ -3577,19 +3577,19 @@
       <c r="S27" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T27" s="56" t="s">
+      <c r="T27" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="U27" s="57" t="s">
+      <c r="U27" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V27" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="W27" s="61">
+      <c r="W27" s="40">
         <v>42322</v>
       </c>
-      <c r="X27" s="61">
+      <c r="X27" s="40">
         <v>42322</v>
       </c>
     </row>
@@ -3647,19 +3647,19 @@
       <c r="S28" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="T28" s="56" t="s">
+      <c r="T28" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="U28" s="57" t="s">
+      <c r="U28" s="36" t="s">
         <v>223</v>
       </c>
       <c r="V28" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W28" s="61">
+      <c r="W28" s="40">
         <v>42325</v>
       </c>
-      <c r="X28" s="61">
+      <c r="X28" s="40">
         <v>42325</v>
       </c>
     </row>
@@ -3717,17 +3717,17 @@
       <c r="S29" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T29" s="56" t="s">
+      <c r="T29" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="U29" s="57" t="s">
+      <c r="U29" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V29" s="26" t="s">
         <v>267</v>
       </c>
       <c r="W29" s="10"/>
-      <c r="X29" s="61">
+      <c r="X29" s="40">
         <v>42355</v>
       </c>
     </row>
@@ -3779,19 +3779,19 @@
       <c r="S30" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T30" s="56" t="s">
+      <c r="T30" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="U30" s="57" t="s">
+      <c r="U30" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V30" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W30" s="61">
+      <c r="W30" s="40">
         <v>42352</v>
       </c>
-      <c r="X30" s="61">
+      <c r="X30" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -3847,19 +3847,19 @@
       <c r="S31" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="T31" s="56" t="s">
+      <c r="T31" s="35" t="s">
         <v>258</v>
       </c>
-      <c r="U31" s="57" t="s">
+      <c r="U31" s="36" t="s">
         <v>246</v>
       </c>
       <c r="V31" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W31" s="61">
+      <c r="W31" s="40">
         <v>42326</v>
       </c>
-      <c r="X31" s="61">
+      <c r="X31" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -3915,19 +3915,19 @@
       <c r="S32" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T32" s="56" t="s">
+      <c r="T32" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="U32" s="57" t="s">
+      <c r="U32" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V32" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W32" s="61">
+      <c r="W32" s="40">
         <v>42353</v>
       </c>
-      <c r="X32" s="61">
+      <c r="X32" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -3985,19 +3985,19 @@
       <c r="S33" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T33" s="56" t="s">
+      <c r="T33" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="U33" s="57" t="s">
+      <c r="U33" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V33" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W33" s="61">
+      <c r="W33" s="40">
         <v>42353</v>
       </c>
-      <c r="X33" s="61">
+      <c r="X33" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -4051,19 +4051,19 @@
       <c r="S34" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T34" s="56" t="s">
+      <c r="T34" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="U34" s="57" t="s">
+      <c r="U34" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V34" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W34" s="61">
+      <c r="W34" s="40">
         <v>42325</v>
       </c>
-      <c r="X34" s="61">
+      <c r="X34" s="40">
         <v>42325</v>
       </c>
       <c r="Y34" s="31" t="s">
@@ -4107,11 +4107,11 @@
       <c r="R35" s="24"/>
       <c r="S35" s="24"/>
       <c r="T35" s="24"/>
-      <c r="U35" s="57"/>
+      <c r="U35" s="36"/>
       <c r="V35" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="W35" s="61">
+      <c r="W35" s="40">
         <v>42321</v>
       </c>
       <c r="X35" s="10"/>
@@ -4162,19 +4162,19 @@
       <c r="S36" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T36" s="56" t="s">
+      <c r="T36" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="U36" s="57" t="s">
+      <c r="U36" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V36" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="W36" s="61">
+      <c r="W36" s="40">
         <v>42329</v>
       </c>
-      <c r="X36" s="61">
+      <c r="X36" s="40">
         <v>42329</v>
       </c>
     </row>
@@ -4226,19 +4226,19 @@
       <c r="S37" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="T37" s="56" t="s">
+      <c r="T37" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="U37" s="57" t="s">
+      <c r="U37" s="36" t="s">
         <v>227</v>
       </c>
       <c r="V37" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="W37" s="61">
+      <c r="W37" s="40">
         <v>42354</v>
       </c>
-      <c r="X37" s="61">
+      <c r="X37" s="40">
         <v>42324</v>
       </c>
     </row>
@@ -5228,6 +5228,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5242,12 +5248,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Observaciones cuaderno de estudio MA_08_05_CO
Revisión del cuaderno de estudio publicado en su primer publicación.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
@@ -444,9 +444,6 @@
   </si>
   <si>
     <t>Resuelve las divisiones de fracciones con polinomios</t>
-  </si>
-  <si>
-    <t>Multiplicación y división de expresiones algebraicas</t>
   </si>
   <si>
     <t>Analiza situaciones de expresiones racionales</t>
@@ -1001,6 +998,9 @@
   </si>
   <si>
     <t>Divide fracciones algebraicas</t>
+  </si>
+  <si>
+    <t>Multiplicación y división de fracciones algebraicas</t>
   </si>
 </sst>
 </file>
@@ -1366,16 +1366,28 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1415,18 +1427,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1735,9 +1735,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P22" sqref="P22"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="47.42578125" defaultRowHeight="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1770,101 +1770,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="3" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="43" t="s">
+      <c r="N1" s="59"/>
+      <c r="O1" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="43" t="s">
+      <c r="P1" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="60" t="s">
+      <c r="Q1" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="61" t="s">
+      <c r="R1" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="60" t="s">
+      <c r="S1" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="59" t="s">
+      <c r="T1" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="58" t="s">
+      <c r="U1" s="43" t="s">
         <v>90</v>
       </c>
       <c r="V1" s="13"/>
     </row>
     <row r="2" spans="1:25" s="3" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="50"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="54"/>
       <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="58"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="43"/>
       <c r="V2" s="13"/>
       <c r="W2" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="X2" s="30" t="s">
         <v>270</v>
-      </c>
-      <c r="X2" s="30" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1878,10 +1878,10 @@
         <v>123</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="23" t="s">
@@ -1894,7 +1894,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K3" s="25" t="s">
         <v>20</v>
@@ -1914,19 +1914,19 @@
         <v>6</v>
       </c>
       <c r="R3" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="S3" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="T3" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="T3" s="35" t="s">
+      <c r="U3" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="U3" s="36" t="s">
-        <v>223</v>
-      </c>
       <c r="V3" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W3" s="40">
         <v>42326</v>
@@ -1946,13 +1946,13 @@
         <v>123</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>131</v>
@@ -1964,7 +1964,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K4" s="25" t="s">
         <v>20</v>
@@ -1977,7 +1977,7 @@
         <v>22</v>
       </c>
       <c r="O4" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P4" s="24" t="s">
         <v>19</v>
@@ -1986,19 +1986,19 @@
         <v>6</v>
       </c>
       <c r="R4" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S4" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="T4" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="T4" s="35" t="s">
+      <c r="U4" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="U4" s="36" t="s">
-        <v>227</v>
-      </c>
       <c r="V4" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
@@ -2014,16 +2014,16 @@
         <v>123</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>157</v>
-      </c>
       <c r="F5" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H5" s="24">
         <v>3</v>
@@ -2032,7 +2032,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K5" s="25" t="s">
         <v>20</v>
@@ -2045,7 +2045,7 @@
         <v>25</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P5" s="24" t="s">
         <v>19</v>
@@ -2054,19 +2054,19 @@
         <v>6</v>
       </c>
       <c r="R5" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S5" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S5" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T5" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U5" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V5" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W5" s="40">
         <v>42320</v>
@@ -2084,14 +2084,14 @@
         <v>123</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H6" s="24">
         <v>4</v>
@@ -2100,7 +2100,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K6" s="25" t="s">
         <v>20</v>
@@ -2113,7 +2113,7 @@
         <v>22</v>
       </c>
       <c r="O6" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P6" s="24" t="s">
         <v>19</v>
@@ -2122,19 +2122,19 @@
         <v>6</v>
       </c>
       <c r="R6" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S6" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S6" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T6" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U6" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V6" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W6" s="40">
         <v>42320</v>
@@ -2152,11 +2152,11 @@
         <v>123</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G7" s="23" t="s">
         <v>132</v>
@@ -2168,7 +2168,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K7" s="25" t="s">
         <v>20</v>
@@ -2181,7 +2181,7 @@
         <v>32</v>
       </c>
       <c r="O7" s="26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P7" s="24" t="s">
         <v>19</v>
@@ -2190,19 +2190,19 @@
         <v>6</v>
       </c>
       <c r="R7" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S7" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S7" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T7" s="35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="U7" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V7" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W7" s="40">
         <v>42320</v>
@@ -2220,10 +2220,10 @@
         <v>123</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G8" s="28" t="s">
         <v>125</v>
@@ -2235,7 +2235,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K8" s="25" t="s">
         <v>20</v>
@@ -2245,10 +2245,10 @@
       </c>
       <c r="M8" s="25"/>
       <c r="N8" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O8" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P8" s="24" t="s">
         <v>19</v>
@@ -2257,19 +2257,19 @@
         <v>6</v>
       </c>
       <c r="R8" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S8" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S8" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T8" s="35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U8" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V8" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W8" s="40">
         <v>42334</v>
@@ -2287,12 +2287,12 @@
         <v>123</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="26"/>
       <c r="G9" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H9" s="24">
         <v>7</v>
@@ -2301,7 +2301,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K9" s="25" t="s">
         <v>20</v>
@@ -2314,7 +2314,7 @@
         <v>39</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P9" s="24" t="s">
         <v>19</v>
@@ -2323,19 +2323,19 @@
         <v>6</v>
       </c>
       <c r="R9" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S9" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S9" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T9" s="35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="U9" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V9" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W9" s="40">
         <v>42354</v>
@@ -2355,14 +2355,14 @@
         <v>123</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>129</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H10" s="24">
         <v>8</v>
@@ -2371,7 +2371,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K10" s="25" t="s">
         <v>20</v>
@@ -2384,7 +2384,7 @@
         <v>119</v>
       </c>
       <c r="O10" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P10" s="24" t="s">
         <v>20</v>
@@ -2393,19 +2393,19 @@
         <v>6</v>
       </c>
       <c r="R10" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S10" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S10" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T10" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="U10" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V10" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W10" s="40">
         <v>42354</v>
@@ -2425,7 +2425,7 @@
         <v>123</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>129</v>
@@ -2441,7 +2441,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K11" s="25" t="s">
         <v>20</v>
@@ -2454,7 +2454,7 @@
         <v>39</v>
       </c>
       <c r="O11" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P11" s="24" t="s">
         <v>19</v>
@@ -2463,19 +2463,19 @@
         <v>6</v>
       </c>
       <c r="R11" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S11" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S11" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T11" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="U11" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V11" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W11" s="40">
         <v>42354</v>
@@ -2495,7 +2495,7 @@
         <v>123</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>129</v>
@@ -2511,7 +2511,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K12" s="25" t="s">
         <v>20</v>
@@ -2524,7 +2524,7 @@
         <v>39</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P12" s="24" t="s">
         <v>19</v>
@@ -2533,19 +2533,19 @@
         <v>6</v>
       </c>
       <c r="R12" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S12" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S12" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T12" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="U12" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V12" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W12" s="40">
         <v>42334</v>
@@ -2565,7 +2565,7 @@
         <v>123</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>129</v>
@@ -2581,7 +2581,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K13" s="25" t="s">
         <v>20</v>
@@ -2594,7 +2594,7 @@
         <v>33</v>
       </c>
       <c r="O13" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P13" s="24" t="s">
         <v>19</v>
@@ -2603,19 +2603,19 @@
         <v>6</v>
       </c>
       <c r="R13" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S13" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S13" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T13" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U13" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V13" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W13" s="40">
         <v>42334</v>
@@ -2635,14 +2635,14 @@
         <v>123</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>129</v>
       </c>
       <c r="F14" s="26"/>
       <c r="G14" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H14" s="24">
         <v>12</v>
@@ -2651,7 +2651,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K14" s="25" t="s">
         <v>20</v>
@@ -2664,7 +2664,7 @@
         <v>29</v>
       </c>
       <c r="O14" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P14" s="24" t="s">
         <v>19</v>
@@ -2673,19 +2673,19 @@
         <v>6</v>
       </c>
       <c r="R14" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S14" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S14" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T14" s="35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="U14" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V14" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W14" s="10"/>
       <c r="X14" s="40">
@@ -2703,7 +2703,7 @@
         <v>123</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>129</v>
@@ -2719,7 +2719,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K15" s="25" t="s">
         <v>20</v>
@@ -2732,7 +2732,7 @@
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P15" s="24" t="s">
         <v>19</v>
@@ -2741,19 +2741,19 @@
         <v>6</v>
       </c>
       <c r="R15" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="S15" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="S15" s="24" t="s">
-        <v>221</v>
-      </c>
       <c r="T15" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U15" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V15" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W15" s="40">
         <v>42326</v>
@@ -2774,14 +2774,14 @@
         <v>123</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F16" s="26"/>
       <c r="G16" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H16" s="24">
         <v>14</v>
@@ -2790,7 +2790,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K16" s="25" t="s">
         <v>20</v>
@@ -2800,10 +2800,10 @@
       </c>
       <c r="M16" s="25"/>
       <c r="N16" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O16" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P16" s="24" t="s">
         <v>19</v>
@@ -2812,19 +2812,19 @@
         <v>6</v>
       </c>
       <c r="R16" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S16" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S16" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T16" s="35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U16" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V16" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W16" s="10"/>
       <c r="X16" s="40">
@@ -2843,16 +2843,16 @@
         <v>123</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>135</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H17" s="24">
         <v>15</v>
@@ -2861,7 +2861,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K17" s="25" t="s">
         <v>20</v>
@@ -2874,7 +2874,7 @@
         <v>39</v>
       </c>
       <c r="O17" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P17" s="24" t="s">
         <v>19</v>
@@ -2883,19 +2883,19 @@
         <v>6</v>
       </c>
       <c r="R17" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S17" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S17" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T17" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U17" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V17" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W17" s="40">
         <v>42352</v>
@@ -2915,14 +2915,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H18" s="24">
         <v>16</v>
@@ -2931,7 +2931,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K18" s="25" t="s">
         <v>20</v>
@@ -2944,7 +2944,7 @@
         <v>39</v>
       </c>
       <c r="O18" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P18" s="24" t="s">
         <v>19</v>
@@ -2953,19 +2953,19 @@
         <v>6</v>
       </c>
       <c r="R18" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S18" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S18" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T18" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U18" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V18" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W18" s="40">
         <v>42352</v>
@@ -2985,7 +2985,7 @@
         <v>123</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="26"/>
@@ -2999,7 +2999,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K19" s="25" t="s">
         <v>20</v>
@@ -3012,7 +3012,7 @@
         <v>29</v>
       </c>
       <c r="O19" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P19" s="24" t="s">
         <v>20</v>
@@ -3021,19 +3021,19 @@
         <v>6</v>
       </c>
       <c r="R19" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S19" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S19" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T19" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U19" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V19" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W19" s="40">
         <v>42352</v>
@@ -3053,7 +3053,7 @@
         <v>123</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="26"/>
@@ -3067,7 +3067,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K20" s="25" t="s">
         <v>20</v>
@@ -3080,7 +3080,7 @@
         <v>39</v>
       </c>
       <c r="O20" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P20" s="24" t="s">
         <v>20</v>
@@ -3089,19 +3089,19 @@
         <v>6</v>
       </c>
       <c r="R20" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S20" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S20" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T20" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U20" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V20" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W20" s="40">
         <v>42352</v>
@@ -3121,7 +3121,7 @@
         <v>123</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="26"/>
@@ -3135,7 +3135,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K21" s="25" t="s">
         <v>20</v>
@@ -3148,7 +3148,7 @@
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P21" s="24" t="s">
         <v>19</v>
@@ -3157,19 +3157,19 @@
         <v>6</v>
       </c>
       <c r="R21" s="24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S21" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="T21" s="35" t="s">
         <v>244</v>
       </c>
-      <c r="T21" s="35" t="s">
+      <c r="U21" s="36" t="s">
         <v>245</v>
       </c>
-      <c r="U21" s="36" t="s">
-        <v>246</v>
-      </c>
       <c r="V21" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W21" s="40">
         <v>42326</v>
@@ -3189,12 +3189,12 @@
         <v>123</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="26"/>
       <c r="G22" s="39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H22" s="24">
         <v>20</v>
@@ -3203,7 +3203,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K22" s="25" t="s">
         <v>20</v>
@@ -3216,7 +3216,7 @@
         <v>121</v>
       </c>
       <c r="O22" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P22" s="24" t="s">
         <v>20</v>
@@ -3225,19 +3225,19 @@
         <v>6</v>
       </c>
       <c r="R22" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S22" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S22" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T22" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="U22" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V22" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W22" s="10"/>
       <c r="X22" s="40">
@@ -3255,11 +3255,11 @@
         <v>123</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>136</v>
@@ -3271,7 +3271,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K23" s="25" t="s">
         <v>20</v>
@@ -3284,7 +3284,7 @@
         <v>39</v>
       </c>
       <c r="O23" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P23" s="24" t="s">
         <v>19</v>
@@ -3293,19 +3293,19 @@
         <v>6</v>
       </c>
       <c r="R23" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S23" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S23" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T23" s="35" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="U23" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V23" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W23" s="10"/>
       <c r="X23" s="40">
@@ -3323,11 +3323,11 @@
         <v>123</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G24" s="23" t="s">
         <v>137</v>
@@ -3339,7 +3339,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K24" s="25" t="s">
         <v>20</v>
@@ -3352,7 +3352,7 @@
         <v>40</v>
       </c>
       <c r="O24" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P24" s="24" t="s">
         <v>20</v>
@@ -3361,25 +3361,25 @@
         <v>6</v>
       </c>
       <c r="R24" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S24" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S24" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T24" s="35" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="U24" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V24" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W24" s="40">
         <v>42322</v>
       </c>
       <c r="X24" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3393,11 +3393,11 @@
         <v>123</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G25" s="23" t="s">
         <v>138</v>
@@ -3409,7 +3409,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K25" s="25" t="s">
         <v>20</v>
@@ -3422,7 +3422,7 @@
         <v>39</v>
       </c>
       <c r="O25" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P25" s="24" t="s">
         <v>19</v>
@@ -3431,19 +3431,19 @@
         <v>6</v>
       </c>
       <c r="R25" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S25" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S25" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T25" s="35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="U25" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V25" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W25" s="40">
         <v>42333</v>
@@ -3464,14 +3464,14 @@
         <v>123</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H26" s="24">
         <v>24</v>
@@ -3480,7 +3480,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K26" s="25" t="s">
         <v>20</v>
@@ -3493,7 +3493,7 @@
         <v>33</v>
       </c>
       <c r="O26" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P26" s="24" t="s">
         <v>19</v>
@@ -3502,19 +3502,19 @@
         <v>6</v>
       </c>
       <c r="R26" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S26" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S26" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T26" s="35" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="U26" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V26" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W26" s="40">
         <v>42321</v>
@@ -3534,11 +3534,11 @@
         <v>123</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G27" s="23" t="s">
         <v>139</v>
@@ -3550,7 +3550,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K27" s="25" t="s">
         <v>20</v>
@@ -3563,7 +3563,7 @@
         <v>39</v>
       </c>
       <c r="O27" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P27" s="24" t="s">
         <v>19</v>
@@ -3572,19 +3572,19 @@
         <v>6</v>
       </c>
       <c r="R27" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S27" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S27" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T27" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U27" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V27" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W27" s="40">
         <v>42322</v>
@@ -3604,14 +3604,14 @@
         <v>123</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G28" s="23" t="s">
-        <v>140</v>
+        <v>289</v>
       </c>
       <c r="H28" s="24">
         <v>26</v>
@@ -3620,7 +3620,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K28" s="25" t="s">
         <v>20</v>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="N28" s="25"/>
       <c r="O28" s="26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P28" s="24" t="s">
         <v>19</v>
@@ -3642,19 +3642,19 @@
         <v>6</v>
       </c>
       <c r="R28" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="S28" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="S28" s="24" t="s">
-        <v>221</v>
-      </c>
       <c r="T28" s="35" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="U28" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V28" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W28" s="40">
         <v>42325</v>
@@ -3674,14 +3674,14 @@
         <v>123</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H29" s="24">
         <v>27</v>
@@ -3690,7 +3690,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K29" s="25" t="s">
         <v>20</v>
@@ -3703,7 +3703,7 @@
         <v>39</v>
       </c>
       <c r="O29" s="26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P29" s="24" t="s">
         <v>19</v>
@@ -3712,19 +3712,19 @@
         <v>6</v>
       </c>
       <c r="R29" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S29" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S29" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T29" s="35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="U29" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V29" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W29" s="10"/>
       <c r="X29" s="40">
@@ -3736,14 +3736,14 @@
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F30" s="26"/>
       <c r="G30" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H30" s="24">
         <v>28</v>
@@ -3752,7 +3752,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K30" s="25" t="s">
         <v>20</v>
@@ -3762,10 +3762,10 @@
       </c>
       <c r="M30" s="25"/>
       <c r="N30" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P30" s="24" t="s">
         <v>19</v>
@@ -3774,19 +3774,19 @@
         <v>6</v>
       </c>
       <c r="R30" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S30" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S30" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T30" s="35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="U30" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V30" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W30" s="40">
         <v>42352</v>
@@ -3806,12 +3806,12 @@
         <v>123</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="26"/>
       <c r="G31" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H31" s="24">
         <v>29</v>
@@ -3820,7 +3820,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K31" s="25" t="s">
         <v>20</v>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="N31" s="25"/>
       <c r="O31" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P31" s="24" t="s">
         <v>19</v>
@@ -3842,19 +3842,19 @@
         <v>6</v>
       </c>
       <c r="R31" s="24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S31" s="24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T31" s="35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U31" s="36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="V31" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W31" s="40">
         <v>42326</v>
@@ -3874,12 +3874,12 @@
         <v>123</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="26"/>
       <c r="G32" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H32" s="24">
         <v>30</v>
@@ -3888,7 +3888,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K32" s="25" t="s">
         <v>20</v>
@@ -3901,7 +3901,7 @@
         <v>39</v>
       </c>
       <c r="O32" s="26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P32" s="24" t="s">
         <v>19</v>
@@ -3910,19 +3910,19 @@
         <v>6</v>
       </c>
       <c r="R32" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S32" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S32" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T32" s="35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U32" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V32" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W32" s="40">
         <v>42353</v>
@@ -3942,14 +3942,14 @@
         <v>123</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F33" s="26"/>
       <c r="G33" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H33" s="24">
         <v>31</v>
@@ -3958,7 +3958,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K33" s="25" t="s">
         <v>20</v>
@@ -3971,7 +3971,7 @@
         <v>52</v>
       </c>
       <c r="O33" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P33" s="24" t="s">
         <v>19</v>
@@ -3980,19 +3980,19 @@
         <v>6</v>
       </c>
       <c r="R33" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S33" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S33" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T33" s="35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="U33" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V33" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W33" s="40">
         <v>42353</v>
@@ -4012,12 +4012,12 @@
         <v>123</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="26"/>
       <c r="G34" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H34" s="24">
         <v>32</v>
@@ -4026,7 +4026,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K34" s="25" t="s">
         <v>20</v>
@@ -4046,19 +4046,19 @@
         <v>6</v>
       </c>
       <c r="R34" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S34" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S34" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T34" s="35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="U34" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V34" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W34" s="40">
         <v>42325</v>
@@ -4067,7 +4067,7 @@
         <v>42325</v>
       </c>
       <c r="Y34" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4093,7 +4093,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K35" s="25" t="s">
         <v>20</v>
@@ -4109,7 +4109,7 @@
       <c r="T35" s="24"/>
       <c r="U35" s="36"/>
       <c r="V35" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W35" s="40">
         <v>42321</v>
@@ -4130,7 +4130,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="26"/>
       <c r="G36" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H36" s="24">
         <v>34</v>
@@ -4139,7 +4139,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K36" s="25" t="s">
         <v>20</v>
@@ -4157,19 +4157,19 @@
         <v>6</v>
       </c>
       <c r="R36" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S36" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S36" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T36" s="35" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U36" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V36" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W36" s="40">
         <v>42329</v>
@@ -4189,12 +4189,12 @@
         <v>123</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="26"/>
       <c r="G37" s="23" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H37" s="24">
         <v>35</v>
@@ -4221,19 +4221,19 @@
         <v>7</v>
       </c>
       <c r="R37" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S37" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="S37" s="24" t="s">
-        <v>225</v>
-      </c>
       <c r="T37" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="U37" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="V37" s="26" t="s">
         <v>266</v>
-      </c>
-      <c r="U37" s="36" t="s">
-        <v>227</v>
-      </c>
-      <c r="V37" s="26" t="s">
-        <v>267</v>
       </c>
       <c r="W37" s="40">
         <v>42354</v>
@@ -5228,12 +5228,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5248,6 +5242,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6018,7 +6018,7 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>

</xml_diff>

<commit_message>
Cambio de nombre de recurso 80
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Escaleta MA_08_05_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="289">
   <si>
     <t>Asignatura</t>
   </si>
@@ -521,9 +521,6 @@
     <t>Dada una expresión racional, los estudiantes deben identificar la o las que son equivalentes, algunas utiliando el cambio de signos y en otras la factorixación.</t>
   </si>
   <si>
-    <t>Se trata de determina cuáles  fracciones algebraicas son equivalentes. Por ejemplo, a la fracción x/x + 1. Las alternativas deben contemplar las distintas posibilidades teniendo el cambio de signo.</t>
-  </si>
-  <si>
     <t>Dar expresiones racionales con términos monomios y el estudiante debe señalar su simplificación</t>
   </si>
   <si>
@@ -651,9 +648,6 @@
   </si>
   <si>
     <t>Actividad para establecer expresiones racionales equivalentes</t>
-  </si>
-  <si>
-    <t>Actividad para identificar equivalencias entre expresiones racionales, teniendo en cuenta el cambio de signo</t>
   </si>
   <si>
     <t>Actividad para practicar la simplificación de epresiones racionales cuyos términos son monomios</t>
@@ -958,9 +952,6 @@
     <t xml:space="preserve">Establece fracciones algebraicas equivalentes </t>
   </si>
   <si>
-    <t>Identifica equivalencias entre fracciones algebraicas</t>
-  </si>
-  <si>
     <t>Actividad para calcular la adición de fracciones algebracicas con monomios en el denominador</t>
   </si>
   <si>
@@ -1001,6 +992,12 @@
   </si>
   <si>
     <t>Refuerza tu aprendizaje: Las operaciones entre fracciones algebraicas</t>
+  </si>
+  <si>
+    <t>Identifica fracciones positivas o negativas</t>
+  </si>
+  <si>
+    <t>Actividad para identificar si las fracciones son positivas o negativas</t>
   </si>
 </sst>
 </file>
@@ -1366,28 +1363,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1427,6 +1412,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1770,101 +1767,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="3" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="41" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="Q1" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="S1" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="T1" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="58" t="s">
         <v>90</v>
       </c>
       <c r="V1" s="13"/>
     </row>
     <row r="2" spans="1:25" s="3" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="54"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="43"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="58"/>
       <c r="V2" s="13"/>
       <c r="W2" s="22" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="X2" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1914,19 +1911,19 @@
         <v>6</v>
       </c>
       <c r="R3" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="T3" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="U3" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="T3" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="U3" s="36" t="s">
-        <v>220</v>
-      </c>
       <c r="V3" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W3" s="40">
         <v>42326</v>
@@ -1964,7 +1961,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K4" s="25" t="s">
         <v>20</v>
@@ -1986,19 +1983,19 @@
         <v>6</v>
       </c>
       <c r="R4" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="S4" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T4" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="U4" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T4" s="35" t="s">
-        <v>223</v>
-      </c>
-      <c r="U4" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V4" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
@@ -2023,7 +2020,7 @@
         <v>149</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H5" s="24">
         <v>3</v>
@@ -2032,7 +2029,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K5" s="25" t="s">
         <v>20</v>
@@ -2054,19 +2051,19 @@
         <v>6</v>
       </c>
       <c r="R5" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S5" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="U5" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T5" s="35" t="s">
-        <v>225</v>
-      </c>
-      <c r="U5" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V5" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W5" s="40">
         <v>42320</v>
@@ -2091,7 +2088,7 @@
         <v>150</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H6" s="24">
         <v>4</v>
@@ -2100,7 +2097,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K6" s="25" t="s">
         <v>20</v>
@@ -2113,7 +2110,7 @@
         <v>22</v>
       </c>
       <c r="O6" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P6" s="24" t="s">
         <v>19</v>
@@ -2122,19 +2119,19 @@
         <v>6</v>
       </c>
       <c r="R6" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S6" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T6" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="U6" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T6" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="U6" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V6" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W6" s="40">
         <v>42320</v>
@@ -2168,7 +2165,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K7" s="25" t="s">
         <v>20</v>
@@ -2190,19 +2187,19 @@
         <v>6</v>
       </c>
       <c r="R7" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S7" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T7" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="U7" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T7" s="35" t="s">
-        <v>227</v>
-      </c>
-      <c r="U7" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V7" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W7" s="40">
         <v>42320</v>
@@ -2235,7 +2232,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K8" s="25" t="s">
         <v>20</v>
@@ -2245,7 +2242,7 @@
       </c>
       <c r="M8" s="25"/>
       <c r="N8" s="25" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O8" s="26" t="s">
         <v>163</v>
@@ -2257,19 +2254,19 @@
         <v>6</v>
       </c>
       <c r="R8" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S8" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T8" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="U8" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T8" s="35" t="s">
-        <v>228</v>
-      </c>
-      <c r="U8" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V8" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W8" s="40">
         <v>42334</v>
@@ -2292,7 +2289,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="26"/>
       <c r="G9" s="23" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H9" s="24">
         <v>7</v>
@@ -2301,7 +2298,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K9" s="25" t="s">
         <v>20</v>
@@ -2323,19 +2320,19 @@
         <v>6</v>
       </c>
       <c r="R9" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S9" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T9" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="U9" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T9" s="35" t="s">
-        <v>229</v>
-      </c>
-      <c r="U9" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V9" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W9" s="40">
         <v>42354</v>
@@ -2362,7 +2359,7 @@
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="23" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="H10" s="24">
         <v>8</v>
@@ -2371,7 +2368,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>209</v>
+        <v>288</v>
       </c>
       <c r="K10" s="25" t="s">
         <v>20</v>
@@ -2383,9 +2380,7 @@
       <c r="N10" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="O10" s="26" t="s">
-        <v>165</v>
-      </c>
+      <c r="O10" s="26"/>
       <c r="P10" s="24" t="s">
         <v>20</v>
       </c>
@@ -2393,19 +2388,19 @@
         <v>6</v>
       </c>
       <c r="R10" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S10" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T10" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="U10" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T10" s="35" t="s">
-        <v>230</v>
-      </c>
-      <c r="U10" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V10" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W10" s="40">
         <v>42354</v>
@@ -2441,7 +2436,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K11" s="25" t="s">
         <v>20</v>
@@ -2454,7 +2449,7 @@
         <v>39</v>
       </c>
       <c r="O11" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P11" s="24" t="s">
         <v>19</v>
@@ -2463,19 +2458,19 @@
         <v>6</v>
       </c>
       <c r="R11" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S11" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T11" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="U11" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T11" s="35" t="s">
-        <v>231</v>
-      </c>
-      <c r="U11" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V11" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W11" s="40">
         <v>42354</v>
@@ -2511,7 +2506,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K12" s="25" t="s">
         <v>20</v>
@@ -2524,7 +2519,7 @@
         <v>39</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P12" s="24" t="s">
         <v>19</v>
@@ -2533,19 +2528,19 @@
         <v>6</v>
       </c>
       <c r="R12" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S12" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T12" s="35" t="s">
+        <v>230</v>
+      </c>
+      <c r="U12" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T12" s="35" t="s">
-        <v>232</v>
-      </c>
-      <c r="U12" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V12" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W12" s="40">
         <v>42334</v>
@@ -2581,7 +2576,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K13" s="25" t="s">
         <v>20</v>
@@ -2594,7 +2589,7 @@
         <v>33</v>
       </c>
       <c r="O13" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P13" s="24" t="s">
         <v>19</v>
@@ -2603,19 +2598,19 @@
         <v>6</v>
       </c>
       <c r="R13" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S13" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T13" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="U13" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T13" s="35" t="s">
-        <v>233</v>
-      </c>
-      <c r="U13" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V13" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W13" s="40">
         <v>42334</v>
@@ -2642,7 +2637,7 @@
       </c>
       <c r="F14" s="26"/>
       <c r="G14" s="23" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H14" s="24">
         <v>12</v>
@@ -2651,7 +2646,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K14" s="25" t="s">
         <v>20</v>
@@ -2664,7 +2659,7 @@
         <v>29</v>
       </c>
       <c r="O14" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P14" s="24" t="s">
         <v>19</v>
@@ -2673,19 +2668,19 @@
         <v>6</v>
       </c>
       <c r="R14" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S14" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T14" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="U14" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T14" s="35" t="s">
-        <v>234</v>
-      </c>
-      <c r="U14" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V14" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W14" s="10"/>
       <c r="X14" s="40">
@@ -2719,7 +2714,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K15" s="25" t="s">
         <v>20</v>
@@ -2732,7 +2727,7 @@
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P15" s="24" t="s">
         <v>19</v>
@@ -2741,19 +2736,19 @@
         <v>6</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S15" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="T15" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="U15" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="T15" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="U15" s="36" t="s">
-        <v>220</v>
-      </c>
       <c r="V15" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W15" s="40">
         <v>42326</v>
@@ -2781,7 +2776,7 @@
       </c>
       <c r="F16" s="26"/>
       <c r="G16" s="28" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H16" s="24">
         <v>14</v>
@@ -2790,7 +2785,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K16" s="25" t="s">
         <v>20</v>
@@ -2800,10 +2795,10 @@
       </c>
       <c r="M16" s="25"/>
       <c r="N16" s="25" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O16" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P16" s="24" t="s">
         <v>19</v>
@@ -2812,19 +2807,19 @@
         <v>6</v>
       </c>
       <c r="R16" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S16" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T16" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="U16" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T16" s="35" t="s">
-        <v>236</v>
-      </c>
-      <c r="U16" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V16" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W16" s="10"/>
       <c r="X16" s="40">
@@ -2852,7 +2847,7 @@
         <v>155</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H17" s="24">
         <v>15</v>
@@ -2861,7 +2856,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="26" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K17" s="25" t="s">
         <v>20</v>
@@ -2874,7 +2869,7 @@
         <v>39</v>
       </c>
       <c r="O17" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P17" s="24" t="s">
         <v>19</v>
@@ -2883,19 +2878,19 @@
         <v>6</v>
       </c>
       <c r="R17" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S17" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T17" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="U17" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T17" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="U17" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V17" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W17" s="40">
         <v>42352</v>
@@ -2922,7 +2917,7 @@
         <v>156</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H18" s="24">
         <v>16</v>
@@ -2931,7 +2926,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="26" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="K18" s="25" t="s">
         <v>20</v>
@@ -2944,7 +2939,7 @@
         <v>39</v>
       </c>
       <c r="O18" s="26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P18" s="24" t="s">
         <v>19</v>
@@ -2953,19 +2948,19 @@
         <v>6</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S18" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T18" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="U18" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T18" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="U18" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V18" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W18" s="40">
         <v>42352</v>
@@ -2999,7 +2994,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="K19" s="25" t="s">
         <v>20</v>
@@ -3012,7 +3007,7 @@
         <v>29</v>
       </c>
       <c r="O19" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P19" s="24" t="s">
         <v>20</v>
@@ -3021,19 +3016,19 @@
         <v>6</v>
       </c>
       <c r="R19" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S19" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T19" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="U19" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T19" s="35" t="s">
-        <v>239</v>
-      </c>
-      <c r="U19" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V19" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W19" s="40">
         <v>42352</v>
@@ -3067,7 +3062,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="K20" s="25" t="s">
         <v>20</v>
@@ -3080,7 +3075,7 @@
         <v>39</v>
       </c>
       <c r="O20" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P20" s="24" t="s">
         <v>20</v>
@@ -3089,19 +3084,19 @@
         <v>6</v>
       </c>
       <c r="R20" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S20" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T20" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="U20" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T20" s="35" t="s">
-        <v>240</v>
-      </c>
-      <c r="U20" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V20" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W20" s="40">
         <v>42352</v>
@@ -3135,7 +3130,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K21" s="25" t="s">
         <v>20</v>
@@ -3148,7 +3143,7 @@
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P21" s="24" t="s">
         <v>19</v>
@@ -3157,19 +3152,19 @@
         <v>6</v>
       </c>
       <c r="R21" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S21" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="T21" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="U21" s="36" t="s">
         <v>241</v>
       </c>
-      <c r="T21" s="35" t="s">
-        <v>242</v>
-      </c>
-      <c r="U21" s="36" t="s">
-        <v>243</v>
-      </c>
       <c r="V21" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W21" s="40">
         <v>42326</v>
@@ -3194,7 +3189,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="26"/>
       <c r="G22" s="39" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H22" s="24">
         <v>20</v>
@@ -3203,7 +3198,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="K22" s="25" t="s">
         <v>20</v>
@@ -3216,7 +3211,7 @@
         <v>121</v>
       </c>
       <c r="O22" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P22" s="24" t="s">
         <v>20</v>
@@ -3225,19 +3220,19 @@
         <v>6</v>
       </c>
       <c r="R22" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S22" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T22" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="U22" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T22" s="35" t="s">
-        <v>244</v>
-      </c>
-      <c r="U22" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V22" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="W22" s="10"/>
       <c r="X22" s="40">
@@ -3271,7 +3266,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K23" s="25" t="s">
         <v>20</v>
@@ -3284,7 +3279,7 @@
         <v>39</v>
       </c>
       <c r="O23" s="26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P23" s="24" t="s">
         <v>19</v>
@@ -3293,19 +3288,19 @@
         <v>6</v>
       </c>
       <c r="R23" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S23" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T23" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="U23" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T23" s="35" t="s">
-        <v>245</v>
-      </c>
-      <c r="U23" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V23" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="W23" s="10"/>
       <c r="X23" s="40">
@@ -3339,7 +3334,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K24" s="25" t="s">
         <v>20</v>
@@ -3352,7 +3347,7 @@
         <v>40</v>
       </c>
       <c r="O24" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P24" s="24" t="s">
         <v>20</v>
@@ -3361,25 +3356,25 @@
         <v>6</v>
       </c>
       <c r="R24" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S24" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T24" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="U24" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T24" s="35" t="s">
-        <v>246</v>
-      </c>
-      <c r="U24" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V24" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="W24" s="40">
         <v>42322</v>
       </c>
       <c r="X24" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3409,7 +3404,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K25" s="25" t="s">
         <v>20</v>
@@ -3422,7 +3417,7 @@
         <v>39</v>
       </c>
       <c r="O25" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P25" s="24" t="s">
         <v>19</v>
@@ -3431,19 +3426,19 @@
         <v>6</v>
       </c>
       <c r="R25" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S25" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T25" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="U25" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T25" s="35" t="s">
-        <v>247</v>
-      </c>
-      <c r="U25" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V25" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="W25" s="40">
         <v>42333</v>
@@ -3471,7 +3466,7 @@
         <v>158</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H26" s="24">
         <v>24</v>
@@ -3480,7 +3475,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K26" s="25" t="s">
         <v>20</v>
@@ -3493,7 +3488,7 @@
         <v>33</v>
       </c>
       <c r="O26" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P26" s="24" t="s">
         <v>19</v>
@@ -3502,19 +3497,19 @@
         <v>6</v>
       </c>
       <c r="R26" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S26" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T26" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="U26" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T26" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="U26" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V26" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="W26" s="40">
         <v>42321</v>
@@ -3550,7 +3545,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K27" s="25" t="s">
         <v>20</v>
@@ -3563,7 +3558,7 @@
         <v>39</v>
       </c>
       <c r="O27" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P27" s="24" t="s">
         <v>19</v>
@@ -3572,19 +3567,19 @@
         <v>6</v>
       </c>
       <c r="R27" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S27" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T27" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="U27" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T27" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="U27" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V27" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="W27" s="40">
         <v>42322</v>
@@ -3608,10 +3603,10 @@
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G28" s="23" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H28" s="24">
         <v>26</v>
@@ -3620,7 +3615,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K28" s="25" t="s">
         <v>20</v>
@@ -3633,7 +3628,7 @@
       </c>
       <c r="N28" s="25"/>
       <c r="O28" s="26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P28" s="24" t="s">
         <v>19</v>
@@ -3642,19 +3637,19 @@
         <v>6</v>
       </c>
       <c r="R28" s="24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S28" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="T28" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="U28" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="T28" s="35" t="s">
-        <v>252</v>
-      </c>
-      <c r="U28" s="36" t="s">
-        <v>220</v>
-      </c>
       <c r="V28" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W28" s="40">
         <v>42325</v>
@@ -3678,7 +3673,7 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G29" s="23" t="s">
         <v>140</v>
@@ -3690,7 +3685,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K29" s="25" t="s">
         <v>20</v>
@@ -3703,7 +3698,7 @@
         <v>39</v>
       </c>
       <c r="O29" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P29" s="24" t="s">
         <v>19</v>
@@ -3712,19 +3707,19 @@
         <v>6</v>
       </c>
       <c r="R29" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S29" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T29" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="U29" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T29" s="35" t="s">
-        <v>253</v>
-      </c>
-      <c r="U29" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V29" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W29" s="10"/>
       <c r="X29" s="40">
@@ -3743,7 +3738,7 @@
       </c>
       <c r="F30" s="26"/>
       <c r="G30" s="23" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H30" s="24">
         <v>28</v>
@@ -3752,7 +3747,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="26" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K30" s="25" t="s">
         <v>20</v>
@@ -3762,10 +3757,10 @@
       </c>
       <c r="M30" s="25"/>
       <c r="N30" s="25" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P30" s="24" t="s">
         <v>19</v>
@@ -3774,19 +3769,19 @@
         <v>6</v>
       </c>
       <c r="R30" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S30" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T30" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="U30" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T30" s="35" t="s">
-        <v>254</v>
-      </c>
-      <c r="U30" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V30" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W30" s="40">
         <v>42352</v>
@@ -3820,7 +3815,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K31" s="25" t="s">
         <v>20</v>
@@ -3833,7 +3828,7 @@
       </c>
       <c r="N31" s="25"/>
       <c r="O31" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P31" s="24" t="s">
         <v>19</v>
@@ -3842,19 +3837,19 @@
         <v>6</v>
       </c>
       <c r="R31" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S31" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="T31" s="35" t="s">
+        <v>253</v>
+      </c>
+      <c r="U31" s="36" t="s">
         <v>241</v>
       </c>
-      <c r="T31" s="35" t="s">
-        <v>255</v>
-      </c>
-      <c r="U31" s="36" t="s">
-        <v>243</v>
-      </c>
       <c r="V31" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W31" s="40">
         <v>42326</v>
@@ -3879,7 +3874,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="26"/>
       <c r="G32" s="23" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H32" s="24">
         <v>30</v>
@@ -3888,7 +3883,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K32" s="25" t="s">
         <v>20</v>
@@ -3901,7 +3896,7 @@
         <v>39</v>
       </c>
       <c r="O32" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P32" s="24" t="s">
         <v>19</v>
@@ -3910,19 +3905,19 @@
         <v>6</v>
       </c>
       <c r="R32" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S32" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T32" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="U32" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T32" s="35" t="s">
-        <v>256</v>
-      </c>
-      <c r="U32" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V32" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W32" s="40">
         <v>42353</v>
@@ -3958,7 +3953,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K33" s="25" t="s">
         <v>20</v>
@@ -3971,7 +3966,7 @@
         <v>52</v>
       </c>
       <c r="O33" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P33" s="24" t="s">
         <v>19</v>
@@ -3980,19 +3975,19 @@
         <v>6</v>
       </c>
       <c r="R33" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S33" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T33" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="U33" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T33" s="35" t="s">
-        <v>257</v>
-      </c>
-      <c r="U33" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V33" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W33" s="40">
         <v>42353</v>
@@ -4017,7 +4012,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="26"/>
       <c r="G34" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H34" s="24">
         <v>32</v>
@@ -4026,7 +4021,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K34" s="25" t="s">
         <v>20</v>
@@ -4046,19 +4041,19 @@
         <v>6</v>
       </c>
       <c r="R34" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S34" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T34" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="U34" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T34" s="35" t="s">
-        <v>258</v>
-      </c>
-      <c r="U34" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V34" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W34" s="40">
         <v>42325</v>
@@ -4067,7 +4062,7 @@
         <v>42325</v>
       </c>
       <c r="Y34" s="31" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4093,7 +4088,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="K35" s="25" t="s">
         <v>20</v>
@@ -4109,7 +4104,7 @@
       <c r="T35" s="24"/>
       <c r="U35" s="36"/>
       <c r="V35" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="W35" s="40">
         <v>42321</v>
@@ -4139,7 +4134,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="26" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K36" s="25" t="s">
         <v>20</v>
@@ -4157,19 +4152,19 @@
         <v>6</v>
       </c>
       <c r="R36" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S36" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T36" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="U36" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T36" s="35" t="s">
-        <v>259</v>
-      </c>
-      <c r="U36" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V36" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="W36" s="40">
         <v>42329</v>
@@ -4189,12 +4184,12 @@
         <v>123</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="26"/>
       <c r="G37" s="23" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H37" s="24">
         <v>35</v>
@@ -4221,19 +4216,19 @@
         <v>7</v>
       </c>
       <c r="R37" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S37" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="T37" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="U37" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="T37" s="35" t="s">
-        <v>263</v>
-      </c>
-      <c r="U37" s="36" t="s">
-        <v>224</v>
-      </c>
       <c r="V37" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W37" s="40">
         <v>42354</v>
@@ -5228,6 +5223,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5242,12 +5243,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6018,7 +6013,7 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>

</xml_diff>